<commit_message>
Allow configuring share class name
</commit_message>
<xml_diff>
--- a/f8621.xlsx
+++ b/f8621.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Lot Details" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t xml:space="preserve">Date: Acquisition</t>
   </si>
@@ -63,13 +63,19 @@
     <t xml:space="preserve">PFIC Reference ID</t>
   </si>
   <si>
+    <t xml:space="preserve">PFIC Share Class</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vanguard FTSE All-World UCITS ETF</t>
   </si>
   <si>
-    <t xml:space="preserve">70 Sir John Rogerson’s Quay, Dublin 2</t>
+    <t xml:space="preserve">70 Sir John Rogerson’s Quay, Dublin Ireland</t>
   </si>
   <si>
     <t xml:space="preserve">VWCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UCITS ETF (USD) Acc.</t>
   </si>
 </sst>
 </file>
@@ -406,10 +412,10 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="A3:D3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -471,20 +477,201 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="7"/>
+      <c r="A3" s="7" t="n">
+        <v>45658</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>50</v>
+      </c>
+      <c r="C3" s="8" t="n">
+        <f aca="false">2500</f>
+        <v>2500</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>1</v>
+      </c>
       <c r="E3" s="7"/>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7"/>
+      <c r="A4" s="7" t="n">
+        <v>45689</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>500</v>
+      </c>
+      <c r="C4" s="8" t="n">
+        <f aca="false">2500</f>
+        <v>2500</v>
+      </c>
+      <c r="D4" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="E4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7"/>
+      <c r="A5" s="7" t="n">
+        <v>45717</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>52</v>
+      </c>
+      <c r="C5" s="8" t="n">
+        <f aca="false">2500</f>
+        <v>2500</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>1</v>
+      </c>
       <c r="E5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7"/>
+      <c r="A6" s="7" t="n">
+        <v>45748</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>53</v>
+      </c>
+      <c r="C6" s="8" t="n">
+        <f aca="false">2500</f>
+        <v>2500</v>
+      </c>
+      <c r="D6" s="9" t="n">
+        <v>1</v>
+      </c>
       <c r="E6" s="7"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="n">
+        <v>45778</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>54</v>
+      </c>
+      <c r="C7" s="8" t="n">
+        <f aca="false">2500</f>
+        <v>2500</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="n">
+        <v>45809</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="C8" s="8" t="n">
+        <f aca="false">2500</f>
+        <v>2500</v>
+      </c>
+      <c r="D8" s="9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="7" t="n">
+        <v>45839</v>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>56</v>
+      </c>
+      <c r="C9" s="8" t="n">
+        <f aca="false">2500</f>
+        <v>2500</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="7" t="n">
+        <v>45870</v>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>57</v>
+      </c>
+      <c r="C10" s="8" t="n">
+        <f aca="false">2500</f>
+        <v>2500</v>
+      </c>
+      <c r="D10" s="9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="7" t="n">
+        <v>45901</v>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>58</v>
+      </c>
+      <c r="C11" s="8" t="n">
+        <f aca="false">2500</f>
+        <v>2500</v>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="7" t="n">
+        <v>45931</v>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>59</v>
+      </c>
+      <c r="C12" s="8" t="n">
+        <f aca="false">2500</f>
+        <v>2500</v>
+      </c>
+      <c r="D12" s="9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="7" t="n">
+        <v>45962</v>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>60</v>
+      </c>
+      <c r="C13" s="8" t="n">
+        <f aca="false">2500</f>
+        <v>2500</v>
+      </c>
+      <c r="D13" s="3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="7" t="n">
+        <v>45992</v>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>61</v>
+      </c>
+      <c r="C14" s="8" t="n">
+        <f aca="false">2500</f>
+        <v>2500</v>
+      </c>
+      <c r="D14" s="9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="7"/>
+      <c r="C15" s="8"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="7"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="9"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="7"/>
+      <c r="C17" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -506,7 +693,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E31" activeCellId="1" sqref="A3:D3 E31"/>
+      <selection pane="topLeft" activeCell="E31" activeCellId="0" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -609,10 +796,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A28" activeCellId="1" sqref="A3:D3 A28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -620,6 +807,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="66.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27.21"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -632,16 +820,22 @@
       <c r="C1" s="14" t="s">
         <v>12</v>
       </c>
+      <c r="D1" s="14" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>